<commit_message>
Completed lab4 may need to fix TODOs
</commit_message>
<xml_diff>
--- a/lab04/data-q1-3.xlsx
+++ b/lab04/data-q1-3.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dudbo\Documents\Code-Projects\COMP3331\lab04\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99B56595-33BA-41A4-990C-8434DC7120AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B212A0C-0075-41BD-A6E4-BCA31BC54BA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2496" yWindow="3168" windowWidth="17280" windowHeight="8880" activeTab="2" xr2:uid="{02BFD1FB-62A2-4081-9DD9-B0B4E602C109}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{02BFD1FB-62A2-4081-9DD9-B0B4E602C109}"/>
   </bookViews>
   <sheets>
     <sheet name="Q3a" sheetId="2" r:id="rId1"/>
     <sheet name="Q3b" sheetId="1" r:id="rId2"/>
     <sheet name="Q3c" sheetId="3" r:id="rId3"/>
+    <sheet name="Ex2" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="32">
   <si>
     <t>Sequence Number</t>
   </si>
@@ -77,6 +78,63 @@
   </si>
   <si>
     <t>Packet Length</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Source IP</t>
+  </si>
+  <si>
+    <t>Destination IP</t>
+  </si>
+  <si>
+    <t>Protocol</t>
+  </si>
+  <si>
+    <t>Info</t>
+  </si>
+  <si>
+    <t>10.9.16.201</t>
+  </si>
+  <si>
+    <t>10.99.6.175</t>
+  </si>
+  <si>
+    <t>TCP</t>
+  </si>
+  <si>
+    <t>50045 &gt; 5000 [SYN] Seq=2818463618 win=8192 MSS=1460</t>
+  </si>
+  <si>
+    <t>5000&gt;50045 [SYN, ACK] Seq=1247095790 Ack=2818463619 win=262144 MSS=1460</t>
+  </si>
+  <si>
+    <t>50045 &gt; 5000 [ACK] Seq=2818463619 Ack=1247095791 win=65535</t>
+  </si>
+  <si>
+    <t>50045 &gt; 5000 [PSH, ACK] Seq=2818463619 Ack=1247095791 win=65535</t>
+  </si>
+  <si>
+    <t>5000&gt;50045 [ACK] Seq=1247095791 Ack=2818463652 win=262096</t>
+  </si>
+  <si>
+    <t>5000&gt;50045 [PSH, ACK] Seq=1247095791 Ack=2818463652 win=262144</t>
+  </si>
+  <si>
+    <t>50045 &gt; 5000 [ACK] Seq=2818463652 Ack=1247095831 win=65535</t>
+  </si>
+  <si>
+    <t>50045 &gt; 5000 [FIN, ACK] Seq=2818463652 Ack=1247095831 win=65535</t>
+  </si>
+  <si>
+    <t>5000 &gt; 50045 [FIN, ACK] Seq=1247095831 Ack=2818463652 win=262144</t>
+  </si>
+  <si>
+    <t>50045 &gt; 5000 [ACK] Seq=2818463652 Ack=1247095832 win=65535</t>
+  </si>
+  <si>
+    <t>5000 &gt; 50045 [ACK] Seq=1247095831 Ack=2818463653 win=262144</t>
   </si>
 </sst>
 </file>
@@ -86,23 +144,35 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Courier New"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF212529"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFAFAFA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -110,13 +180,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFDEE2E6"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFDEE2E6"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFDEE2E6"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFDEE2E6"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -802,8 +890,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0475C7F3-D29A-402C-B348-1E70AD25F338}">
   <dimension ref="A2:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1162,4 +1250,228 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04831258-62D1-43BB-BE05-8C9DE994D589}">
+  <dimension ref="A1:E13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="6.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="60" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="2">
+        <v>295</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="2">
+        <v>296</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="2">
+        <v>297</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="2">
+        <v>298</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="2">
+        <v>301</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="2">
+        <v>302</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="2">
+        <v>303</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="2">
+        <v>304</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="2">
+        <v>305</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="2">
+        <v>306</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="2">
+        <v>308</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>